<commit_message>
Apun ko puraa DHAK DHAK ho gayelaa
</commit_message>
<xml_diff>
--- a/src/assets/MultiuserTemplate.xlsx
+++ b/src/assets/MultiuserTemplate.xlsx
@@ -264,11 +264,11 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>
@@ -280,6 +280,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Almighty Pushhhhh . . !!!
</commit_message>
<xml_diff>
--- a/src/assets/MultiuserTemplate.xlsx
+++ b/src/assets/MultiuserTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">FIRSTNAME</t>
   </si>
@@ -31,12 +31,18 @@
     <t xml:space="preserve">PHONE</t>
   </si>
   <si>
+    <t xml:space="preserve">GENDER</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMAIL</t>
   </si>
   <si>
     <t xml:space="preserve">DOB</t>
   </si>
   <si>
+    <t xml:space="preserve">GOVT_ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMPCODE</t>
   </si>
   <si>
@@ -55,18 +61,27 @@
     <t xml:space="preserve">DEPARTMENT</t>
   </si>
   <si>
+    <t xml:space="preserve">PERMISSION</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biswajit</t>
   </si>
   <si>
     <t xml:space="preserve">Sahoo</t>
   </si>
   <si>
+    <t xml:space="preserve">MALE / FEMALE</t>
+  </si>
+  <si>
     <t xml:space="preserve">A@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">DD-MM-YYYY</t>
   </si>
   <si>
+    <t xml:space="preserve">Aadhar / PAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">E754567</t>
   </si>
   <si>
@@ -80,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES / NO</t>
   </si>
 </sst>
 </file>
@@ -262,25 +280,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,52 +323,70 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1111111</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,8 +397,10 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
@@ -372,8 +410,10 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
@@ -383,8 +423,10 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="K5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -394,9 +436,11 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
@@ -406,9 +450,11 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
@@ -418,9 +464,11 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
@@ -430,9 +478,11 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
@@ -442,13 +492,15 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="A@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="A@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>